<commit_message>
serenity screenplay login functionality
</commit_message>
<xml_diff>
--- a/serenityBDDFreamework/src/test/resources/TestDataExcel/ExcelData.xlsx
+++ b/serenityBDDFreamework/src/test/resources/TestDataExcel/ExcelData.xlsx
@@ -3,14 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\serenityBDDFreamework\src\test\resources\TestDataExcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14652" windowHeight="3192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18144" windowHeight="2244"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -28,17 +32,17 @@
     <t>password</t>
   </si>
   <si>
-    <t>akhil.thokala@emlen.io</t>
+    <t>jhansi+admadv@finlink.de</t>
   </si>
   <si>
-    <t>qa1@emlen</t>
+    <t>vikas+admadv@finlink.de</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,6 +52,28 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -76,9 +102,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -360,15 +393,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -380,27 +414,30 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="3">
+        <v>12345678</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>30303030</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>